<commit_message>
add current boundary map, update student number
</commit_message>
<xml_diff>
--- a/resources/student_number.xlsx
+++ b/resources/student_number.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Elementary School" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>timberline:</t>
   </si>
   <si>
-    <t>1/3=&gt;stroller</t>
-  </si>
-  <si>
     <t xml:space="preserve">cedar park: </t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>Five Oak</t>
   </si>
   <si>
-    <t>2/3-&gt;Medow Park</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
@@ -203,6 +197,12 @@
   </si>
   <si>
     <t>Mountainside</t>
+  </si>
+  <si>
+    <t>1/2=&gt;stroller</t>
+  </si>
+  <si>
+    <t>1/2-&gt;Medow Park</t>
   </si>
 </sst>
 </file>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,13 +695,13 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -736,10 +736,10 @@
         <v>28</v>
       </c>
       <c r="L2">
-        <v>2131</v>
+        <v>2210</v>
       </c>
       <c r="M2">
-        <v>1065</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -829,16 +829,16 @@
         <v>727</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
         <v>29</v>
       </c>
       <c r="L5">
-        <v>2200</v>
+        <v>2082</v>
       </c>
       <c r="M5">
-        <v>1100</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -957,7 +957,7 @@
         <v>349</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9">
         <v>1914</v>
@@ -1111,7 +1111,7 @@
         <v>359</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L14">
         <v>1958</v>
@@ -1265,13 +1265,13 @@
         <v>634</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L19">
-        <v>2130</v>
+        <v>2249</v>
       </c>
       <c r="M19">
-        <v>1065</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>714</v>
       </c>
       <c r="J22" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1393,13 +1393,13 @@
         <v>528</v>
       </c>
       <c r="K23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L23">
-        <v>2145</v>
+        <v>2026</v>
       </c>
       <c r="M23">
-        <v>1072</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,12 @@
         <v>590</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <f>SUM(I6:I8)</f>
+        <v>1719</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1481,7 +1486,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1">
         <v>6</v>
@@ -1493,12 +1498,12 @@
         <v>8</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>415</v>
@@ -1518,7 +1523,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>111</v>
@@ -1535,7 +1540,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>287</v>
@@ -1555,7 +1560,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>63</v>
@@ -1572,7 +1577,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>294</v>
@@ -1589,7 +1594,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>213</v>
@@ -1609,7 +1614,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>34</v>
@@ -1626,7 +1631,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>230</v>
@@ -1646,7 +1651,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>68</v>
@@ -1663,7 +1668,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11">
         <v>292</v>
@@ -1680,7 +1685,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>247</v>
@@ -1700,7 +1705,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>27</v>
@@ -1711,7 +1716,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>316</v>
@@ -1735,15 +1740,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1">
         <v>9</v>
@@ -1758,12 +1763,12 @@
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2">
         <v>619</v>
@@ -1783,7 +1788,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>541</v>
@@ -1803,7 +1808,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>373</v>
@@ -1823,7 +1828,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>446</v>
@@ -1843,7 +1848,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>415</v>
@@ -1863,7 +1868,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>448</v>

</xml_diff>